<commit_message>
Minor changes and new functions
</commit_message>
<xml_diff>
--- a/+DataKit/ressources/validQualityFlags.xlsx
+++ b/+DataKit/ressources/validQualityFlags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/David/Dropbox/David/Syncing/MATLAB/toolboxes/+DataKit/ressources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC46A76-BD69-8948-953B-3EAB68029D2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7FA418-44D5-2741-95A0-40E08CBDD4A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18460" yWindow="15740" windowWidth="26840" windowHeight="13060" xr2:uid="{B22FD432-52D0-7045-8884-EBF804A53727}"/>
+    <workbookView xWindow="2400" yWindow="8500" windowWidth="26840" windowHeight="9140" xr2:uid="{B22FD432-52D0-7045-8884-EBF804A53727}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>QualityFlag</t>
   </si>
@@ -45,13 +37,22 @@
   </si>
   <si>
     <t>Value below the detection limit (&lt; 1µM)</t>
+  </si>
+  <si>
+    <t>%u16</t>
+  </si>
+  <si>
+    <t>%s</t>
+  </si>
+  <si>
+    <t>&lt;noIssue&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -396,18 +397,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6022B0-A14B-764F-B9D3-FEB0D7A4EDF7}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,19 +416,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>